<commit_message>
Ubah text jadi num
</commit_message>
<xml_diff>
--- a/DEMATEL/data.xlsx
+++ b/DEMATEL/data.xlsx
@@ -9,21 +9,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Nilai UAS</t>
+    <t>Berat</t>
   </si>
   <si>
-    <t>Nilai UTS</t>
+    <t>Tinggi</t>
   </si>
   <si>
-    <t>Tugas</t>
-  </si>
-  <si>
-    <t>Praktikum</t>
-  </si>
-  <si>
-    <t>Tes</t>
+    <t>Panjang</t>
   </si>
 </sst>
 </file>
@@ -68,14 +62,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:D4"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="4" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="6" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -89,12 +81,6 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -104,16 +90,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
         <v>4</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -121,7 +101,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -129,70 +109,18 @@
       <c r="D3">
         <v>3</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
       <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
         <v>0</v>
       </c>
     </row>

</xml_diff>